<commit_message>
SC and EB added
</commit_message>
<xml_diff>
--- a/data/auxiliary/MPWSP_Screen.xlsx
+++ b/data/auxiliary/MPWSP_Screen.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianpg/Documents/ProjectsLocal/Marina_Borehole_Geophysics/data/auxiliary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724F0C0E-0350-B247-BC10-CA2CA27FA37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAF19CA-E84A-3941-80EA-8CC58BB41D3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1180" windowWidth="24440" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="540" windowWidth="17320" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="90">
   <si>
     <t>Hole ID</t>
   </si>
@@ -97,15 +97,230 @@
   </si>
   <si>
     <t>GroupedAquifer</t>
+  </si>
+  <si>
+    <t>Screen_Top_ft</t>
+  </si>
+  <si>
+    <t>Screen_Bottom_ft</t>
+  </si>
+  <si>
+    <t>PR-1</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>ML-1</t>
+  </si>
+  <si>
+    <t>113.5</t>
+  </si>
+  <si>
+    <t>118.5</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>ML-2</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>ML-3</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>ML-4</t>
+  </si>
+  <si>
+    <t>163.5</t>
+  </si>
+  <si>
+    <t>173.5</t>
+  </si>
+  <si>
+    <t>74.5</t>
+  </si>
+  <si>
+    <t>84.5</t>
+  </si>
+  <si>
+    <t>ML-6</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>MDW-1</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>CX-B1</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>CX-B2</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>CX-B4</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t>248</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>180/400-Foot Aquitard</t>
+  </si>
+  <si>
+    <t>Screen_Len_ft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -120,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,12 +343,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,15 +662,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,13 +690,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -455,14 +718,26 @@
       <c r="D2">
         <v>99.669600000000003</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <f>C2/0.3048</f>
+        <v>276.99999999999994</v>
+      </c>
+      <c r="F2">
+        <f>D2/0.3048</f>
+        <v>327</v>
+      </c>
+      <c r="G2">
+        <f>F2-E2</f>
+        <v>50.000000000000057</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -475,14 +750,26 @@
       <c r="D3">
         <v>68.58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <f t="shared" ref="E3:F22" si="0">C3/0.3048</f>
+        <v>115</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>224.99999999999997</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G53" si="1">F3-E3</f>
+        <v>109.99999999999997</v>
+      </c>
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -495,14 +782,26 @@
       <c r="D4">
         <v>28.956</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>54.999999999999993</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>40.000000000000007</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -515,14 +814,26 @@
       <c r="D5">
         <v>100.584</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -535,14 +846,26 @@
       <c r="D6">
         <v>79.248000000000005</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -555,14 +878,26 @@
       <c r="D7">
         <v>30.48</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -575,14 +910,26 @@
       <c r="D8">
         <v>132.58799999999999</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>395</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>434.99999999999994</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>39.999999999999943</v>
+      </c>
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -595,14 +942,26 @@
       <c r="D9">
         <v>94.488</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -615,14 +974,26 @@
       <c r="D10">
         <v>25.298400000000001</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -635,14 +1006,26 @@
       <c r="D11">
         <v>99.06</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -655,14 +1038,26 @@
       <c r="D12">
         <v>64.007999999999996</v>
       </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>209.99999999999997</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>59.999999999999972</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -675,14 +1070,26 @@
       <c r="D13">
         <v>18.288</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -695,14 +1102,26 @@
       <c r="D14">
         <v>105.15600000000001</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
         <v>15</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -715,14 +1134,26 @@
       <c r="D15">
         <v>67.055999999999997</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>219.99999999999997</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>89.999999999999972</v>
+      </c>
+      <c r="H15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -735,14 +1166,26 @@
       <c r="D16">
         <v>24.384</v>
       </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -755,14 +1198,26 @@
       <c r="D17">
         <v>106.68</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -775,14 +1230,26 @@
       <c r="D18">
         <v>65.531999999999996</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>89.999999999999972</v>
+      </c>
+      <c r="H18" t="s">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -795,14 +1262,26 @@
       <c r="D19">
         <v>24.384</v>
       </c>
-      <c r="E19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -815,14 +1294,26 @@
       <c r="D20">
         <v>119.7864</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>352.99999999999994</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>393</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>40.000000000000057</v>
+      </c>
+      <c r="H20" t="s">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -835,14 +1326,26 @@
       <c r="D21">
         <v>68.58</v>
       </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>224.99999999999997</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>79.999999999999972</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -855,10 +1358,1014 @@
       <c r="D22">
         <v>33.527999999999999</v>
       </c>
-      <c r="E22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>109.99999999999999</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>79.999999999999986</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f>E23*0.3048</f>
+        <v>57.912000000000006</v>
+      </c>
+      <c r="D23">
+        <f>F23*0.3048</f>
+        <v>60.96</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:C53" si="2">E24*0.3048</f>
+        <v>38.1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D53" si="3">F24*0.3048</f>
+        <v>41.148000000000003</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>34.594799999999999</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>36.1188</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>27.432000000000002</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>30.48</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="2">
+        <v>100</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>50.901600000000002</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>53.949600000000004</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>27.432000000000002</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>30.48</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="2">
+        <v>100</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>54.864000000000004</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>57.912000000000006</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>31.394400000000001</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>34.442399999999999</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>49.834800000000001</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>52.882800000000003</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>22.707600000000003</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>25.755600000000001</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>46.329599999999999</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>49.377600000000001</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>30.48</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>33.527999999999999</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>72.2376</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>75.285600000000002</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>56.997600000000006</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>60.0456</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>46.329599999999999</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>49.377600000000001</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>18.288</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>21.336000000000002</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>83.515200000000007</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>86.563200000000009</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>72.2376</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>75.285600000000002</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>55.473600000000005</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>58.521600000000007</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="3">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>40.843200000000003</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>43.891200000000005</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="3">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>25.603200000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>28.651200000000003</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="3">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>15.5448</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>18.5928</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H44" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>65.531999999999996</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>68.58</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>49.072800000000001</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>52.120800000000003</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>31.699200000000001</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>34.747199999999999</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="3">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>16.763999999999999</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>19.812000000000001</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H48" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>93.268799999999999</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>96.316800000000001</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>75.590400000000002</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="3"/>
+        <v>78.638400000000004</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="3">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>47.244</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="3"/>
+        <v>50.292000000000002</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="3">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>33.527999999999999</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>36.576000000000001</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>17.6784</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>20.726400000000002</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H53" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>